<commit_message>
excel and ppt(image spotlight):: by sergio giraldo @ 20230307T1310CET, gpg signed
</commit_message>
<xml_diff>
--- a/excel/horas de trabalho.xlsx
+++ b/excel/horas de trabalho.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/GK47LX/source/office/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61A27BF8-2B03-674F-B797-B8968B2F5DAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6052B270-E812-3549-80F5-E381D3DEF629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20440" xr2:uid="{7F259FA3-8C20-4DB0-80F6-590C9FAB135E}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
   <si>
     <t>day</t>
   </si>
@@ -176,13 +176,19 @@
     <t>workdays does not consider the initial day in the math</t>
   </si>
   <si>
-    <t>workdays consider weekends and holidays. There is also the INTL version</t>
-  </si>
-  <si>
     <t>RESULT</t>
   </si>
   <si>
     <t>HOLIDAYS</t>
+  </si>
+  <si>
+    <t>to make a column of dates skipping days and/or holidays</t>
+  </si>
+  <si>
+    <t>this below are only mondays and wednesdays, skipping holidays</t>
+  </si>
+  <si>
+    <t>workdays consider weekends and holidays. There is also the INTL version above</t>
   </si>
 </sst>
 </file>
@@ -195,9 +201,16 @@
     <numFmt numFmtId="166" formatCode="mmmm\ \'yy"/>
     <numFmt numFmtId="167" formatCode="d"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -624,159 +637,185 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="7" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="2" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="6" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -836,6 +875,50 @@
         <a:xfrm>
           <a:off x="13919200" y="7239000"/>
           <a:ext cx="2768600" cy="2146300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>279400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>292100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6C89CB3-24C8-763C-BCE0-6A5AD20F957D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20383500" y="838200"/>
+          <a:ext cx="3048000" cy="2476500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1144,10 +1227,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1140815C-AC11-8E43-94BC-BD9CBE060858}">
-  <dimension ref="A1:X24"/>
+  <dimension ref="A1:AB24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+      <selection activeCell="V4" sqref="V4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -1173,43 +1256,52 @@
     <col min="22" max="22" width="15.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="30.5" style="2" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="10.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="16384" width="8.83203125" style="2"/>
+    <col min="25" max="27" width="8.83203125" style="2"/>
+    <col min="28" max="28" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="31"/>
       <c r="B1" s="4"/>
-      <c r="C1" s="69" t="s">
+      <c r="C1" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
       <c r="J1" s="48"/>
       <c r="K1" s="48"/>
       <c r="L1" s="48"/>
       <c r="M1" s="48"/>
       <c r="N1" s="48"/>
       <c r="O1" s="35"/>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="V1" s="76" t="s">
+        <v>40</v>
+      </c>
+      <c r="W1" s="77"/>
+      <c r="X1" s="77"/>
+      <c r="Y1" s="77"/>
+      <c r="Z1" s="78"/>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" s="36"/>
       <c r="B2" s="30"/>
       <c r="C2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="70" t="s">
+      <c r="D2" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="71"/>
-      <c r="F2" s="70" t="s">
+      <c r="E2" s="69"/>
+      <c r="F2" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="72"/>
-      <c r="H2" s="71"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="69"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
@@ -1220,8 +1312,15 @@
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
       <c r="R2" s="5"/>
-    </row>
-    <row r="3" spans="1:24" ht="25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="V2" s="79" t="s">
+        <v>41</v>
+      </c>
+      <c r="W2" s="80"/>
+      <c r="X2" s="80"/>
+      <c r="Y2" s="80"/>
+      <c r="Z2" s="81"/>
+    </row>
+    <row r="3" spans="1:28" ht="25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="36"/>
       <c r="B3" s="30"/>
       <c r="C3" s="7"/>
@@ -1251,12 +1350,20 @@
       <c r="S3" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="T3" s="65" t="s">
-        <v>39</v>
-      </c>
-      <c r="U3" s="55"/>
-    </row>
-    <row r="4" spans="1:24" ht="25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="T3" s="63" t="s">
+        <v>38</v>
+      </c>
+      <c r="U3" s="72"/>
+      <c r="V3" s="82">
+        <v>44349</v>
+      </c>
+      <c r="W3" s="83"/>
+      <c r="X3" s="83"/>
+      <c r="Y3" s="83"/>
+      <c r="Z3" s="84"/>
+      <c r="AB3" s="74"/>
+    </row>
+    <row r="4" spans="1:28" ht="25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="36"/>
       <c r="B4" s="11" t="s">
         <v>7</v>
@@ -1294,22 +1401,33 @@
       <c r="O4" s="49"/>
       <c r="P4" s="14"/>
       <c r="Q4" s="5"/>
-      <c r="R4" s="56">
+      <c r="R4" s="55">
         <v>44958</v>
       </c>
       <c r="S4" s="54">
         <v>1</v>
       </c>
-      <c r="T4" s="57">
+      <c r="T4" s="56">
         <f>R4+S4</f>
         <v>44959</v>
       </c>
-      <c r="U4" s="51" t="str" cm="1">
+      <c r="U4" s="73" t="str" cm="1">
         <f t="array" aca="1" ref="U4:U7" ca="1">_xlfn.FORMULATEXT(T4:T7)</f>
         <v>=R4+S4</v>
       </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="V4" s="82">
+        <f>WORKDAY.INTL(V3,1,"0101111",$P$17:$P$19)</f>
+        <v>44354</v>
+      </c>
+      <c r="W4" s="83" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(V4)</f>
+        <v>=WORKDAY.INTL(V3;1;"0101111";$P$17:$P$19)</v>
+      </c>
+      <c r="X4" s="83"/>
+      <c r="Y4" s="83"/>
+      <c r="Z4" s="84"/>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" s="36"/>
       <c r="B5" s="15" t="s">
         <v>8</v>
@@ -1345,22 +1463,33 @@
       <c r="O5" s="49"/>
       <c r="P5" s="14"/>
       <c r="Q5" s="14"/>
-      <c r="R5" s="56">
+      <c r="R5" s="55">
         <v>44959</v>
       </c>
       <c r="S5" s="54">
         <v>-1</v>
       </c>
-      <c r="T5" s="57">
+      <c r="T5" s="56">
         <f t="shared" ref="T5:T7" si="1">R5+S5</f>
         <v>44958</v>
       </c>
-      <c r="U5" s="51" t="str">
+      <c r="U5" s="73" t="str">
         <f ca="1"/>
         <v>=R5+S5</v>
       </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="V5" s="82">
+        <f t="shared" ref="V5:V11" si="2">WORKDAY.INTL(V4,1,"0101111",$P$17:$P$19)</f>
+        <v>44356</v>
+      </c>
+      <c r="W5" s="83" t="str">
+        <f t="shared" ref="W5:W11" ca="1" si="3">_xlfn.FORMULATEXT(V5)</f>
+        <v>=WORKDAY.INTL(V4;1;"0101111";$P$17:$P$19)</v>
+      </c>
+      <c r="X5" s="83"/>
+      <c r="Y5" s="83"/>
+      <c r="Z5" s="84"/>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6" s="36"/>
       <c r="B6" s="15" t="s">
         <v>9</v>
@@ -1396,22 +1525,33 @@
       <c r="O6" s="49"/>
       <c r="P6" s="14"/>
       <c r="Q6" s="5"/>
-      <c r="R6" s="56">
+      <c r="R6" s="55">
         <v>44962</v>
       </c>
       <c r="S6" s="54">
         <v>10</v>
       </c>
-      <c r="T6" s="57">
+      <c r="T6" s="56">
         <f t="shared" si="1"/>
         <v>44972</v>
       </c>
-      <c r="U6" s="51" t="str">
+      <c r="U6" s="73" t="str">
         <f ca="1"/>
         <v>=R6+S6</v>
       </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="V6" s="82">
+        <f t="shared" si="2"/>
+        <v>44361</v>
+      </c>
+      <c r="W6" s="83" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>=WORKDAY.INTL(V5;1;"0101111";$P$17:$P$19)</v>
+      </c>
+      <c r="X6" s="83"/>
+      <c r="Y6" s="83"/>
+      <c r="Z6" s="84"/>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" s="36"/>
       <c r="B7" s="15" t="s">
         <v>10</v>
@@ -1447,22 +1587,33 @@
       <c r="O7" s="49"/>
       <c r="P7" s="14"/>
       <c r="Q7" s="5"/>
-      <c r="R7" s="56">
+      <c r="R7" s="55">
         <v>44968</v>
       </c>
       <c r="S7" s="54">
         <v>-10</v>
       </c>
-      <c r="T7" s="57">
+      <c r="T7" s="56">
         <f t="shared" si="1"/>
         <v>44958</v>
       </c>
-      <c r="U7" s="51" t="str">
+      <c r="U7" s="73" t="str">
         <f ca="1"/>
         <v>=R7+S7</v>
       </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="V7" s="82">
+        <f t="shared" si="2"/>
+        <v>44363</v>
+      </c>
+      <c r="W7" s="83" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>=WORKDAY.INTL(V6;1;"0101111";$P$17:$P$19)</v>
+      </c>
+      <c r="X7" s="83"/>
+      <c r="Y7" s="83"/>
+      <c r="Z7" s="84"/>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A8" s="36"/>
       <c r="B8" s="15" t="s">
         <v>11</v>
@@ -1499,14 +1650,25 @@
       <c r="O8" s="49"/>
       <c r="P8" s="14"/>
       <c r="Q8" s="5"/>
-      <c r="R8" s="60" t="s">
+      <c r="R8" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="S8" s="61"/>
-      <c r="T8" s="58"/>
-      <c r="U8" s="59"/>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="S8" s="59"/>
+      <c r="T8" s="57"/>
+      <c r="U8" s="57"/>
+      <c r="V8" s="82">
+        <f t="shared" si="2"/>
+        <v>44368</v>
+      </c>
+      <c r="W8" s="83" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>=WORKDAY.INTL(V7;1;"0101111";$P$17:$P$19)</v>
+      </c>
+      <c r="X8" s="83"/>
+      <c r="Y8" s="83"/>
+      <c r="Z8" s="84"/>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9" s="36"/>
       <c r="B9" s="15" t="s">
         <v>12</v>
@@ -1544,8 +1706,19 @@
       <c r="P9" s="5"/>
       <c r="Q9" s="5"/>
       <c r="R9" s="5"/>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="V9" s="82">
+        <f t="shared" si="2"/>
+        <v>44370</v>
+      </c>
+      <c r="W9" s="83" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>=WORKDAY.INTL(V8;1;"0101111";$P$17:$P$19)</v>
+      </c>
+      <c r="X9" s="83"/>
+      <c r="Y9" s="83"/>
+      <c r="Z9" s="84"/>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A10" s="36"/>
       <c r="B10" s="20" t="s">
         <v>13</v>
@@ -1568,8 +1741,19 @@
       <c r="P10" s="5"/>
       <c r="Q10" s="5"/>
       <c r="R10" s="5"/>
-    </row>
-    <row r="11" spans="1:24" ht="25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="V10" s="82">
+        <f t="shared" si="2"/>
+        <v>44377</v>
+      </c>
+      <c r="W10" s="83" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>=WORKDAY.INTL(V9;1;"0101111";$P$17:$P$19)</v>
+      </c>
+      <c r="X10" s="83"/>
+      <c r="Y10" s="83"/>
+      <c r="Z10" s="84"/>
+    </row>
+    <row r="11" spans="1:28" ht="25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="36"/>
       <c r="B11" s="26" t="s">
         <v>6</v>
@@ -1593,8 +1777,19 @@
       <c r="P11" s="5"/>
       <c r="Q11" s="5"/>
       <c r="R11" s="5"/>
-    </row>
-    <row r="12" spans="1:24" ht="25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="V11" s="85">
+        <f t="shared" si="2"/>
+        <v>44382</v>
+      </c>
+      <c r="W11" s="86" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>=WORKDAY.INTL(V10;1;"0101111";$P$17:$P$19)</v>
+      </c>
+      <c r="X11" s="86"/>
+      <c r="Y11" s="86"/>
+      <c r="Z11" s="87"/>
+    </row>
+    <row r="12" spans="1:28" ht="25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="45"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -1611,22 +1806,22 @@
       <c r="N12" s="46"/>
       <c r="O12" s="47"/>
     </row>
-    <row r="13" spans="1:24" ht="25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:28" ht="25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="T13" s="53" t="s">
         <v>32</v>
       </c>
       <c r="U13" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="V13" s="65" t="s">
+      <c r="V13" s="63" t="s">
+        <v>38</v>
+      </c>
+      <c r="W13" s="54"/>
+      <c r="X13" s="60" t="s">
         <v>39</v>
       </c>
-      <c r="W13" s="54"/>
-      <c r="X13" s="62" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" ht="122" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:28" ht="122" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="31"/>
       <c r="B14" s="32" t="s">
         <v>18</v>
@@ -1654,13 +1849,13 @@
       <c r="O14" s="34"/>
       <c r="P14" s="34"/>
       <c r="Q14" s="35"/>
-      <c r="T14" s="56">
+      <c r="T14" s="55">
         <v>44958</v>
       </c>
       <c r="U14" s="54">
         <v>3</v>
       </c>
-      <c r="V14" s="57">
+      <c r="V14" s="56">
         <f>WORKDAY(T14,U14,$X$14:$X$17)</f>
         <v>44964</v>
       </c>
@@ -1668,11 +1863,11 @@
         <f ca="1">_xlfn.FORMULATEXT(V14)</f>
         <v>=WORKDAY(T14;U14;$X$14:$X$17)</v>
       </c>
-      <c r="X14" s="63">
+      <c r="X14" s="61">
         <v>44959</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A15" s="36"/>
       <c r="B15" s="37">
         <v>44349</v>
@@ -1693,38 +1888,38 @@
         <v>5</v>
       </c>
       <c r="G15" s="5"/>
-      <c r="H15" s="73">
+      <c r="H15" s="71">
         <f>EOMONTH(DATE(2021,5,1),0)+1</f>
         <v>44348</v>
       </c>
-      <c r="I15" s="73"/>
-      <c r="J15" s="73"/>
-      <c r="K15" s="73"/>
-      <c r="L15" s="73"/>
-      <c r="M15" s="73"/>
-      <c r="N15" s="73"/>
+      <c r="I15" s="71"/>
+      <c r="J15" s="71"/>
+      <c r="K15" s="71"/>
+      <c r="L15" s="71"/>
+      <c r="M15" s="71"/>
+      <c r="N15" s="71"/>
       <c r="O15" s="5"/>
       <c r="P15" s="5"/>
       <c r="Q15" s="38"/>
-      <c r="T15" s="56">
+      <c r="T15" s="55">
         <v>44960</v>
       </c>
       <c r="U15" s="54">
         <v>-1</v>
       </c>
-      <c r="V15" s="57">
-        <f t="shared" ref="V15:V17" si="2">WORKDAY(T15,U15,$X$14:$X$17)</f>
+      <c r="V15" s="56">
+        <f t="shared" ref="V15:V17" si="4">WORKDAY(T15,U15,$X$14:$X$17)</f>
         <v>44958</v>
       </c>
       <c r="W15" s="51" t="str">
-        <f t="shared" ref="W15:W17" ca="1" si="3">_xlfn.FORMULATEXT(V15)</f>
+        <f t="shared" ref="W15:W17" ca="1" si="5">_xlfn.FORMULATEXT(V15)</f>
         <v>=WORKDAY(T15;U15;$X$14:$X$17)</v>
       </c>
-      <c r="X15" s="63">
+      <c r="X15" s="61">
         <v>44966</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A16" s="36"/>
       <c r="B16" s="37">
         <v>44371</v>
@@ -1771,21 +1966,21 @@
         <v>28</v>
       </c>
       <c r="Q16" s="38"/>
-      <c r="T16" s="56">
+      <c r="T16" s="55">
         <v>44963</v>
       </c>
       <c r="U16" s="54">
         <v>10</v>
       </c>
-      <c r="V16" s="57">
-        <f t="shared" si="2"/>
+      <c r="V16" s="56">
+        <f t="shared" si="4"/>
         <v>44978</v>
       </c>
       <c r="W16" s="51" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="5"/>
         <v>=WORKDAY(T16;U16;$X$14:$X$17)</v>
       </c>
-      <c r="X16" s="64"/>
+      <c r="X16" s="62"/>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A17" s="36"/>
@@ -1822,21 +2017,21 @@
         <v>44350</v>
       </c>
       <c r="Q17" s="38"/>
-      <c r="T17" s="56">
+      <c r="T17" s="55">
         <v>44970</v>
       </c>
       <c r="U17" s="54">
         <v>-6</v>
       </c>
-      <c r="V17" s="57">
-        <f t="shared" si="2"/>
+      <c r="V17" s="56">
+        <f t="shared" si="4"/>
         <v>44958</v>
       </c>
       <c r="W17" s="51" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="5"/>
         <v>=WORKDAY(T17;U17;$X$14:$X$17)</v>
       </c>
-      <c r="X17" s="64"/>
+      <c r="X17" s="62"/>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18" s="36"/>
@@ -1872,13 +2067,13 @@
         <v>44375</v>
       </c>
       <c r="Q18" s="38"/>
-      <c r="T18" s="66" t="s">
-        <v>38</v>
-      </c>
-      <c r="U18" s="67"/>
-      <c r="V18" s="67"/>
-      <c r="W18" s="67"/>
-      <c r="X18" s="68"/>
+      <c r="T18" s="75" t="s">
+        <v>42</v>
+      </c>
+      <c r="U18" s="65"/>
+      <c r="V18" s="65"/>
+      <c r="W18" s="65"/>
+      <c r="X18" s="66"/>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A19" s="36"/>
@@ -1914,13 +2109,13 @@
         <v>44376</v>
       </c>
       <c r="Q19" s="38"/>
-      <c r="T19" s="66" t="s">
+      <c r="T19" s="64" t="s">
         <v>37</v>
       </c>
-      <c r="U19" s="67"/>
-      <c r="V19" s="67"/>
-      <c r="W19" s="67"/>
-      <c r="X19" s="68"/>
+      <c r="U19" s="65"/>
+      <c r="V19" s="65"/>
+      <c r="W19" s="65"/>
+      <c r="X19" s="66"/>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A20" s="36"/>
@@ -2052,13 +2247,15 @@
       <c r="Q24" s="47"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
     <mergeCell ref="T18:X18"/>
     <mergeCell ref="T19:X19"/>
     <mergeCell ref="C1:I1"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:H2"/>
     <mergeCell ref="H15:N15"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="V2:Z2"/>
   </mergeCells>
   <conditionalFormatting sqref="H15">
     <cfRule type="expression" dxfId="0" priority="1">

</xml_diff>